<commit_message>
add a method for interploting missing data and rename the data file for dropna.py
</commit_message>
<xml_diff>
--- a/DataCleanning/uid.xlsx
+++ b/DataCleanning/uid.xlsx
@@ -1,36 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="135" windowWidth="19395" windowHeight="7605"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
-    <t>序号</t>
+    <t>uid</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>用户A</t>
+    <t>regit_date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>用户B</t>
+    <t>gender</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>用户C</t>
+    <t>age</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>income</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -38,29 +50,41 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
-      <family val="2"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -73,23 +97,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -385,163 +405,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>235.83</v>
-      </c>
-      <c r="C2" s="1">
-        <v>324.02999999999997</v>
+        <v>81200457</v>
+      </c>
+      <c r="B2" s="2">
+        <v>42673</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D2" s="1">
-        <v>478.32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>236.27</v>
-      </c>
-      <c r="C3" s="1">
-        <v>325.63</v>
+        <v>81201135</v>
+      </c>
+      <c r="B3" s="2">
+        <v>42682</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D3" s="1">
-        <v>515.45000000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1">
+        <v>10300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>238.05</v>
-      </c>
-      <c r="C4" s="1">
-        <v>328.08</v>
-      </c>
-      <c r="D4" s="1">
-        <v>517.09</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+        <v>80043782</v>
+      </c>
+      <c r="B4" s="2">
+        <v>42656</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>235.9</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>84639281</v>
+      </c>
+      <c r="B5" s="2">
+        <v>42842</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D5" s="1">
-        <v>514.89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
+        <v>73499801</v>
+      </c>
+      <c r="B6" s="2">
+        <v>42450</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>72399510</v>
+      </c>
+      <c r="B7" s="2">
+        <v>42387</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>63881943</v>
+      </c>
+      <c r="B8" s="2">
+        <v>42284</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>35442690</v>
+      </c>
+      <c r="B9" s="2">
+        <v>42104</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
-        <v>236.76</v>
-      </c>
-      <c r="C6" s="1">
-        <v>268.82</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="1">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>77638351</v>
+      </c>
+      <c r="B10" s="2">
+        <v>42563</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1">
-        <v>404.04</v>
-      </c>
-      <c r="D7" s="1">
-        <v>486.09</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>237.41</v>
-      </c>
-      <c r="C8" s="1">
-        <v>391.26</v>
-      </c>
-      <c r="D8" s="1">
-        <v>516.23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>238.65</v>
-      </c>
-      <c r="C9" s="1">
-        <v>380.81</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>237.61</v>
-      </c>
-      <c r="C10" s="1">
-        <v>388.02</v>
-      </c>
       <c r="D10" s="1">
-        <v>435.35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+        <v>25</v>
+      </c>
+      <c r="E10" s="1">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>238.03</v>
-      </c>
-      <c r="C11" s="1">
-        <v>206.43</v>
+        <v>85200189</v>
+      </c>
+      <c r="B11" s="2">
+        <v>42873</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D11" s="1">
-        <v>487.67500000000001</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E11" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -555,6 +610,7 @@
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>